<commit_message>
- Fixed duplicate scene importing
</commit_message>
<xml_diff>
--- a/CG - Final Assignment - Evaluation Form.xlsx
+++ b/CG - Final Assignment - Evaluation Form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Cpp\School\final_assignment_computer_graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{853750BA-4522-4E9A-AF83-F49B2800840B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6F9B7C-3C20-48CE-88D1-DCC91A257834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4875" yWindow="4980" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation form" sheetId="1" r:id="rId1"/>
@@ -1283,8 +1283,8 @@
   </sheetPr>
   <dimension ref="B2:M37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="E17" s="24">
         <f>IF(COUNTIF($E$12:$E$14,"x")&gt;0,1,MAX(SUM(E20:E36)/10,1))</f>
-        <v>1</v>
+        <v>6.7</v>
       </c>
       <c r="F17" s="37"/>
       <c r="G17" s="38"/>
@@ -1452,7 +1452,9 @@
       <c r="C20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="5">
+        <v>10</v>
+      </c>
       <c r="F20" s="9"/>
       <c r="H20" s="19" t="s">
         <v>79</v>
@@ -1474,7 +1476,9 @@
       <c r="C21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6">
+        <v>5</v>
+      </c>
       <c r="F21" s="10"/>
       <c r="H21" s="12" t="s">
         <v>73</v>
@@ -1496,7 +1500,9 @@
       <c r="C22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="6"/>
+      <c r="E22" s="6">
+        <v>5</v>
+      </c>
       <c r="F22" s="10"/>
       <c r="H22" s="12" t="s">
         <v>35</v>
@@ -1518,7 +1524,9 @@
       <c r="C23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6">
+        <v>10</v>
+      </c>
       <c r="F23" s="10"/>
       <c r="H23" s="12" t="s">
         <v>38</v>
@@ -1540,7 +1548,9 @@
       <c r="C24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="6"/>
+      <c r="E24" s="6">
+        <v>7</v>
+      </c>
       <c r="F24" s="10"/>
       <c r="H24" s="12" t="s">
         <v>23</v>
@@ -1562,7 +1572,9 @@
       <c r="C25" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="6">
+        <v>5</v>
+      </c>
       <c r="F25" s="10"/>
       <c r="H25" s="12" t="s">
         <v>12</v>
@@ -1584,7 +1596,9 @@
       <c r="C26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="6">
+        <v>5</v>
+      </c>
       <c r="F26" s="10"/>
       <c r="H26" s="12" t="s">
         <v>13</v>
@@ -1606,7 +1620,9 @@
       <c r="C27" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="7">
+        <v>5</v>
+      </c>
       <c r="F27" s="11"/>
       <c r="H27" s="15" t="s">
         <v>70</v>
@@ -1652,7 +1668,9 @@
       <c r="C30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5">
+        <v>10</v>
+      </c>
       <c r="F30" s="9"/>
       <c r="H30" s="12" t="s">
         <v>27</v>
@@ -1674,7 +1692,9 @@
       <c r="C31" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="7"/>
+      <c r="E31" s="7">
+        <v>5</v>
+      </c>
       <c r="F31" s="11"/>
       <c r="H31" s="15" t="s">
         <v>86</v>
@@ -1720,7 +1740,9 @@
       <c r="C34" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="5">
+        <v>0</v>
+      </c>
       <c r="F34" s="9"/>
       <c r="H34" s="12" t="s">
         <v>51</v>
@@ -1740,7 +1762,9 @@
       <c r="C35" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="6"/>
+      <c r="E35" s="6">
+        <v>0</v>
+      </c>
       <c r="F35" s="10"/>
       <c r="H35" s="12" t="s">
         <v>60</v>
@@ -1758,7 +1782,9 @@
       <c r="C36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="7"/>
+      <c r="E36" s="7">
+        <v>0</v>
+      </c>
       <c r="F36" s="11"/>
       <c r="H36" s="15" t="s">
         <v>53</v>
@@ -1808,6 +1834,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="22" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="140c34f89499b6d54cc6b190361ded78">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a368ba0ea1756c322acb58be99b19eb5" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2079,26 +2125,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <SharedWithUsers xmlns="7178be8b-d0ef-4995-97d9-396f4bad9a56">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2109,6 +2135,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCBC19EF-510F-4DD0-BF64-52716B5001B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2128,24 +2172,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{704D0896-41A1-4D8E-B2B4-DAF4537F2CEF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95702B07-5163-4733-93F0-15C1454EB37E}">
   <ds:schemaRefs>

</xml_diff>